<commit_message>
Reset repo: Uploading TestApp and Spreadsheet only
</commit_message>
<xml_diff>
--- a/master_spreadsheet_25_26_summer.xlsx
+++ b/master_spreadsheet_25_26_summer.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29602"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yilia/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yilia/Desktop/GI-Test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB66EF27-EC7B-4301-BC63-5AF66F27EC21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DAB8DB-4D8B-844E-81DF-578C62B324C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="4020" windowWidth="21600" windowHeight="11300" firstSheet="2" activeTab="2" xr2:uid="{44EEA75D-67FD-4678-9465-A167448191E0}"/>
+    <workbookView xWindow="3820" yWindow="4900" windowWidth="21720" windowHeight="8360" activeTab="2" xr2:uid="{44EEA75D-67FD-4678-9465-A167448191E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined Price List 25-26 Sum" sheetId="8" r:id="rId1"/>
     <sheet name="Processing Charges 25-26 Sum" sheetId="9" r:id="rId2"/>
     <sheet name="Config 25-26 Sum" sheetId="4" r:id="rId3"/>
-    <sheet name="Discount 25-26 Sum" sheetId="10" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Combined Price List 25-26 Sum'!$A$1:$G$18</definedName>
@@ -112,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="63">
   <si>
     <t>Product Code</t>
   </si>
@@ -225,18 +224,6 @@
     <t>KBrand 775 from 10x</t>
   </si>
   <si>
-    <t>Service #1</t>
-  </si>
-  <si>
-    <t>Service Fee</t>
-  </si>
-  <si>
-    <t>Service #2</t>
-  </si>
-  <si>
-    <t>Service #3</t>
-  </si>
-  <si>
     <t>Group</t>
   </si>
   <si>
@@ -291,9 +278,6 @@
     <t>Surcharge Amount</t>
   </si>
   <si>
-    <t>Surcharge Order</t>
-  </si>
-  <si>
     <t>PRICE_LIST</t>
   </si>
   <si>
@@ -316,18 +300,6 @@
   </si>
   <si>
     <t>Commercial Non-PRJ</t>
-  </si>
-  <si>
-    <t>Discount Brand</t>
-  </si>
-  <si>
-    <t>Discount Amount</t>
-  </si>
-  <si>
-    <t>Xenium​</t>
-  </si>
-  <si>
-    <t>GEM-X Single Immune Profiling Solution v3​</t>
   </si>
 </sst>
 </file>
@@ -338,7 +310,7 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="[$$-C09]#,##0.00"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -366,7 +338,6 @@
       <sz val="11"/>
       <color rgb="FF242424"/>
       <name val="Aptos Narrow"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -415,32 +386,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Aptos Display"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF262626"/>
-      <name val="Aptos Display"/>
-      <scheme val="major"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -455,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -473,7 +425,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -494,14 +445,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -874,53 +820,53 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C563ED3B-1FC1-41B6-96FD-AB3B357F4708}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScale="67" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.625" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" customWidth="1"/>
     <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.125" customWidth="1"/>
+    <col min="4" max="4" width="36.1640625" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
-    <col min="6" max="6" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="10" customFormat="1" ht="49.5">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:9" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="33">
+    <row r="2" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -938,7 +884,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="29.25">
+    <row r="3" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -958,7 +904,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="29.25">
+    <row r="4" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -975,7 +921,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="29.25">
+    <row r="5" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -992,7 +938,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="29.25">
+    <row r="6" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -1009,7 +955,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="33">
+    <row r="7" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1027,7 +973,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1045,7 +991,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1062,43 +1008,43 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15">
+    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>30</v>
       </c>
       <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="11"/>
+      <c r="E10" s="10"/>
       <c r="F10" s="1">
         <v>4500</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15">
+    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>32</v>
       </c>
       <c r="B11" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>33</v>
       </c>
       <c r="D11" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="11"/>
+      <c r="E11" s="10"/>
       <c r="F11" s="1">
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="29.25">
+    <row r="12" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1116,10 +1062,10 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1">
+    <row r="13" spans="1:9" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:9" ht="15">
+    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>36</v>
       </c>
@@ -1134,7 +1080,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>36</v>
       </c>
@@ -1148,37 +1094,37 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15">
+    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="11"/>
+      <c r="E16" s="10"/>
       <c r="F16" s="1">
         <v>4500</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="15">
+    <row r="17" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>33</v>
       </c>
       <c r="D17" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="11"/>
+      <c r="E17" s="10"/>
       <c r="F17" s="1">
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="29.25">
+    <row r="18" spans="2:6" ht="32" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>36</v>
       </c>
@@ -1193,32 +1139,8 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="2:6" s="9" customFormat="1" ht="13.5" customHeight="1">
-      <c r="C19" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" s="9" customFormat="1" ht="13.5" customHeight="1">
-      <c r="C20" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" s="9" customFormat="1" ht="13.5" customHeight="1">
-      <c r="C21" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="4:4" ht="15">
-      <c r="D39" s="4"/>
+    <row r="36" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="D36" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G18" xr:uid="{23277D7F-FEEB-4763-B364-04AA243FCA2B}">
@@ -1240,130 +1162,130 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{890F6873-EDC7-4BE5-9189-E951DA1318D3}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView zoomScale="94" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.375" customWidth="1"/>
-    <col min="2" max="2" width="73.375" customWidth="1"/>
-    <col min="3" max="3" width="33.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.625" customWidth="1"/>
-    <col min="5" max="5" width="11.25" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" customWidth="1"/>
+    <col min="2" max="2" width="73.33203125" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B2" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="10" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="13">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15">
-      <c r="A2" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="14">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15">
-      <c r="A3" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>48</v>
-      </c>
       <c r="D3" s="8"/>
-      <c r="E3" s="14">
+      <c r="E3" s="13">
         <v>5000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15">
-      <c r="A4" s="13" t="s">
-        <v>45</v>
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="13">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="13">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="13">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="14">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15">
-      <c r="A5" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="B7" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="14">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15">
-      <c r="A6" s="13" t="s">
+      <c r="C7" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="14">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15">
-      <c r="A7" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>55</v>
-      </c>
       <c r="D7" s="8"/>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <v>5000</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="E9" s="1"/>
     </row>
@@ -1375,155 +1297,98 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D55C99-92A7-4BC5-9E4D-8387E6974F28}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.25" customWidth="1"/>
-    <col min="2" max="2" width="20.25" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16.5">
-      <c r="A2" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="C2" s="5">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.5">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C3" s="5">
         <v>1.3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C4" s="5">
         <v>1</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+    </row>
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C5">
         <v>1.3</v>
       </c>
-      <c r="D5" s="20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+    </row>
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C6">
         <v>1.45</v>
       </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+    </row>
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C7">
         <v>1.2</v>
       </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="10"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E225A74-4726-489B-BA52-DC430EC611A1}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="22.125" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15">
-      <c r="A1" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.25">
-      <c r="A2" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="29.25">
-      <c r="A3" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3">
-        <v>0.3</v>
-      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1812,13 +1677,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8371111F-EFF7-47C6-8985-0F43994E666C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8371111F-EFF7-47C6-8985-0F43994E666C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{343B393C-CAC2-4750-ACA8-00CCC9C377F8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{343B393C-CAC2-4750-ACA8-00CCC9C377F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="17163bdb-27fe-447c-a7bb-3ea6416b971c"/>
+    <ds:schemaRef ds:uri="451c1f4f-a267-451c-a3af-09c2fa4691f1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC068CDB-1687-487F-8048-C21B0C8EEFAA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC068CDB-1687-487F-8048-C21B0C8EEFAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="17163bdb-27fe-447c-a7bb-3ea6416b971c"/>
+    <ds:schemaRef ds:uri="451c1f4f-a267-451c-a3af-09c2fa4691f1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update master spreadsheet to new 25-26 summer template
</commit_message>
<xml_diff>
--- a/master_spreadsheet_25_26_summer.xlsx
+++ b/master_spreadsheet_25_26_summer.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yilia/Desktop/GI-Test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ysche\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DAB8DB-4D8B-844E-81DF-578C62B324C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E2AD726-FCB5-4004-B499-D314F00F6CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3820" yWindow="4900" windowWidth="21720" windowHeight="8360" activeTab="2" xr2:uid="{44EEA75D-67FD-4678-9465-A167448191E0}"/>
+    <workbookView xWindow="-57720" yWindow="-2700" windowWidth="29040" windowHeight="15720" xr2:uid="{44EEA75D-67FD-4678-9465-A167448191E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined Price List 25-26 Sum" sheetId="8" r:id="rId1"/>
     <sheet name="Processing Charges 25-26 Sum" sheetId="9" r:id="rId2"/>
     <sheet name="Config 25-26 Sum" sheetId="4" r:id="rId3"/>
+    <sheet name="Discount 25-26 Sum" sheetId="10" r:id="rId4"/>
+    <sheet name="Surcharge Editing Page" sheetId="11" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Combined Price List 25-26 Sum'!$A$1:$G$18</definedName>
@@ -111,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="86">
   <si>
     <t>Product Code</t>
   </si>
@@ -140,6 +142,9 @@
     <t>Item Specific Discount</t>
   </si>
   <si>
+    <t>Platform</t>
+  </si>
+  <si>
     <t>10X-1000263</t>
   </si>
   <si>
@@ -152,12 +157,18 @@
     <t>Library &amp; Gel Bead Kit</t>
   </si>
   <si>
+    <t>Type1;Type2</t>
+  </si>
+  <si>
     <t>10X-1000265</t>
   </si>
   <si>
     <t>Chromium Next GEM Single Cell 5' Kit v2, 4 rxns</t>
   </si>
   <si>
+    <t>Type1;Type2;Type3</t>
+  </si>
+  <si>
     <t>10X-1000190</t>
   </si>
   <si>
@@ -167,6 +178,9 @@
     <t>Additional Library Kits</t>
   </si>
   <si>
+    <t>Type1</t>
+  </si>
+  <si>
     <t>10X-1000541</t>
   </si>
   <si>
@@ -179,6 +193,9 @@
     <t>Chromium Single Cell</t>
   </si>
   <si>
+    <t>ALL_PLATFORMS</t>
+  </si>
+  <si>
     <t>10X-1234572</t>
   </si>
   <si>
@@ -203,18 +220,27 @@
     <t>Chromium GEM-X Single Cell 5' Kit v3, 16 rxns</t>
   </si>
   <si>
+    <t>Type1;Type3</t>
+  </si>
+  <si>
     <t>10X-1000712</t>
   </si>
   <si>
     <t>Chromium GEM-X Single Cell 5' Kit v3, 48 rxns</t>
   </si>
   <si>
+    <t>Type2</t>
+  </si>
+  <si>
     <t>10X-1000694</t>
   </si>
   <si>
     <t>Library Construction Kit C, 16 rxns</t>
   </si>
   <si>
+    <t>Type2;Type3</t>
+  </si>
+  <si>
     <t>10X-1000703</t>
   </si>
   <si>
@@ -224,6 +250,12 @@
     <t>KBrand 775 from 10x</t>
   </si>
   <si>
+    <t>Type3</t>
+  </si>
+  <si>
+    <t>Type2;Type1</t>
+  </si>
+  <si>
     <t>Group</t>
   </si>
   <si>
@@ -300,17 +332,57 @@
   </si>
   <si>
     <t>Commercial Non-PRJ</t>
+  </si>
+  <si>
+    <t>Discount Supplier</t>
+  </si>
+  <si>
+    <t>Discount Label</t>
+  </si>
+  <si>
+    <t>Discount Amount</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Single-Cell Discount</t>
+  </si>
+  <si>
+    <t>Spatial Discount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEM-X </t>
+  </si>
+  <si>
+    <t>Gem-X1 Discount</t>
+  </si>
+  <si>
+    <t>Gem-X2 Discount</t>
+  </si>
+  <si>
+    <t>Surcharges</t>
+  </si>
+  <si>
+    <t>Consumables</t>
+  </si>
+  <si>
+    <t>Ext. Commercial Non-PRJ</t>
+  </si>
+  <si>
+    <t>Processing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="[$$-C09]#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,6 +410,7 @@
       <sz val="11"/>
       <color rgb="FF242424"/>
       <name val="Aptos Narrow"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -386,6 +459,85 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF262626"/>
+      <name val="Aptos Display"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF262626"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF262626"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -407,7 +559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -445,9 +597,34 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -820,24 +997,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C563ED3B-1FC1-41B6-96FD-AB3B357F4708}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView zoomScale="67" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.6640625" customWidth="1"/>
+    <col min="2" max="2" width="43.625" customWidth="1"/>
     <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.1640625" customWidth="1"/>
+    <col min="4" max="4" width="36.125" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
-    <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="9" customFormat="1" ht="69.95">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -865,37 +1042,43 @@
       <c r="I1" s="18" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J1" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="29.1">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="1">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="29.1">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="F3" s="1">
         <v>100</v>
@@ -903,243 +1086,288 @@
       <c r="G3" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="29.1">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="29.1">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F5" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="29.1">
       <c r="A6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="F6" s="1">
         <v>104</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="29.1">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="1">
         <v>1000</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="J7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="1">
         <v>5000</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="J8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="14.1">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F9" s="1">
         <v>5000</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="29.1">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="1">
         <v>4500</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="14.45">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="29.1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="J12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="14.1" hidden="1">
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="15">
       <c r="B14" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="1">
         <v>5000</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="J14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="14.1">
       <c r="B15" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F15" s="1">
         <v>5000</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="29.1">
       <c r="B16" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="1">
         <v>4500</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="J16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="14.45">
       <c r="B17" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="J17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="29.1">
       <c r="B18" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="36" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="J18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" ht="15">
       <c r="D36" s="4"/>
     </row>
   </sheetData>
@@ -1160,132 +1388,153 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{890F6873-EDC7-4BE5-9189-E951DA1318D3}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView zoomScale="94" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="34.33203125" customWidth="1"/>
-    <col min="2" max="2" width="73.33203125" customWidth="1"/>
-    <col min="3" max="3" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" customWidth="1"/>
+    <col min="1" max="1" width="34.375" customWidth="1"/>
+    <col min="2" max="2" width="73.375" customWidth="1"/>
+    <col min="3" max="3" width="33.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.625" customWidth="1"/>
+    <col min="5" max="5" width="11.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15">
       <c r="A1" s="11" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D1" s="17" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15">
       <c r="A2" s="12" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="13">
         <v>4000</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="12" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="13">
         <v>5000</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15">
       <c r="A4" s="12" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="13">
         <v>500</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15">
       <c r="A5" s="12" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="13">
         <v>1500</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15">
       <c r="A6" s="12" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="E6" s="13">
         <v>2500</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15">
       <c r="A7" s="12" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="13">
         <v>5000</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="14.1">
       <c r="A8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="14.1">
       <c r="A9" s="1"/>
       <c r="E9" s="1"/>
     </row>
@@ -1297,98 +1546,377 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D55C99-92A7-4BC5-9E4D-8387E6974F28}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.25" customWidth="1"/>
+    <col min="2" max="2" width="20.375" customWidth="1"/>
+    <col min="3" max="3" width="20.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="14.1">
+      <c r="A1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="18"/>
+    </row>
+    <row r="2" spans="1:4" ht="14.1">
       <c r="A2" s="5" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C2" s="5">
+        <f>'Surcharge Editing Page'!C4</f>
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="14.1">
       <c r="A3" s="5" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C3" s="5">
+        <f>'Surcharge Editing Page'!D4</f>
         <v>1.3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="14.1">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C4" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="14.1">
       <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5">
+        <f>'Surcharge Editing Page'!D8*'Config 25-26 Sum'!C4</f>
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="14.1">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6">
+        <f>C5*'Surcharge Editing Page'!E8</f>
+        <v>1.885</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="14.1">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7">
+        <f>C6*'Surcharge Editing Page'!F8</f>
+        <v>2.262</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+    </row>
+    <row r="13" spans="1:4" ht="14.1"/>
+    <row r="16" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A16" s="19"/>
+    </row>
+    <row r="17" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A17" s="19"/>
+    </row>
+    <row r="19" spans="1:4" ht="27" customHeight="1">
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+    </row>
+    <row r="20" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E225A74-4726-489B-BA52-DC430EC611A1}">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView zoomScale="197" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.1"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="17.375" customWidth="1"/>
+    <col min="3" max="3" width="15.75" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="33" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15">
+      <c r="A1" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:5" ht="15">
+      <c r="A2" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5">
+      <c r="B2" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="23">
+        <v>0.15</v>
+      </c>
+      <c r="D2" s="32">
+        <v>45610</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15">
+      <c r="A3" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="23">
+        <v>0.2</v>
+      </c>
+      <c r="D3" s="32">
+        <v>46009</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15">
+      <c r="A4" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="23">
+        <v>0.18</v>
+      </c>
+      <c r="D4" s="32">
+        <v>46034</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15">
+      <c r="A5" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="D5" s="32">
+        <v>46034</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15">
+      <c r="A6" s="19"/>
+    </row>
+    <row r="7" spans="1:5" ht="15">
+      <c r="A7" s="19"/>
+    </row>
+    <row r="8" spans="1:5" ht="15">
+      <c r="A8" s="19"/>
+    </row>
+    <row r="9" spans="1:5" ht="15">
+      <c r="A9" s="19"/>
+    </row>
+    <row r="10" spans="1:5" ht="15">
+      <c r="A10" s="19"/>
+    </row>
+    <row r="11" spans="1:5" ht="15">
+      <c r="A11" s="19"/>
+    </row>
+    <row r="12" spans="1:5" ht="15">
+      <c r="A12" s="19"/>
+    </row>
+    <row r="13" spans="1:5" ht="15">
+      <c r="A13" s="19"/>
+    </row>
+    <row r="14" spans="1:5" ht="15">
+      <c r="A14" s="19"/>
+    </row>
+    <row r="15" spans="1:5" ht="15">
+      <c r="A15" s="19"/>
+    </row>
+    <row r="16" spans="1:5" ht="15">
+      <c r="A16" s="19"/>
+    </row>
+    <row r="17" spans="1:1" ht="15">
+      <c r="A17" s="19"/>
+    </row>
+    <row r="18" spans="1:1" ht="15">
+      <c r="A18" s="19"/>
+    </row>
+    <row r="19" spans="1:1" ht="15">
+      <c r="A19" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9210A67B-8F15-4C29-B057-A84A9BFC79C1}">
+  <dimension ref="A2:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.1"/>
+  <cols>
+    <col min="1" max="1" width="19.625" customWidth="1"/>
+    <col min="2" max="2" width="6.625" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="11.75" customWidth="1"/>
+    <col min="6" max="6" width="12.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" ht="26.1">
+      <c r="A2" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+    </row>
+    <row r="3" spans="1:6" ht="15">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+    </row>
+    <row r="4" spans="1:6" ht="15">
+      <c r="A4" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D4" s="23">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6">
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+    </row>
+    <row r="5" spans="1:6" ht="15">
+      <c r="A5" s="28"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+    </row>
+    <row r="6" spans="1:6" ht="15">
+      <c r="A6" s="28"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+    </row>
+    <row r="7" spans="1:6" ht="43.5">
+      <c r="A7" s="28"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15">
+      <c r="A8" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23">
+        <v>1</v>
+      </c>
+      <c r="D8" s="23">
+        <v>1.3</v>
+      </c>
+      <c r="E8" s="23">
         <v>1.45</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7">
+      <c r="F8" s="23">
         <v>1.2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
+    <row r="9" spans="1:6">
+      <c r="A9" s="20"/>
+    </row>
+    <row r="10" spans="1:6" ht="15">
+      <c r="A10" s="20"/>
+      <c r="D10" s="21"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1405,19 +1933,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="17163bdb-27fe-447c-a7bb-3ea6416b971c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="451c1f4f-a267-451c-a3af-09c2fa4691f1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009F2383067D6EEE4E8ACEA30962E5DE00" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7cc0d0870af9c458a3e9395faf3ddb47">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="17163bdb-27fe-447c-a7bb-3ea6416b971c" xmlns:ns3="451c1f4f-a267-451c-a3af-09c2fa4691f1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7ae48021bdb2fffb49c59b252a7010f2" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009F2383067D6EEE4E8ACEA30962E5DE00" ma:contentTypeVersion="22" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0ccd53f3dd568480f5d3153c07534dba">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="17163bdb-27fe-447c-a7bb-3ea6416b971c" xmlns:ns3="451c1f4f-a267-451c-a3af-09c2fa4691f1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0211ec30299ddd16592819eab657260f" ns2:_="" ns3:_="">
     <xsd:import namespace="17163bdb-27fe-447c-a7bb-3ea6416b971c"/>
     <xsd:import namespace="451c1f4f-a267-451c-a3af-09c2fa4691f1"/>
     <xsd:element name="properties">
@@ -1444,6 +1961,7 @@
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceBillingMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:Notes" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1533,6 +2051,13 @@
     <xsd:element name="MediaServiceBillingMetadata" ma:index="26" nillable="true" ma:displayName="MediaServiceBillingMetadata" ma:hidden="true" ma:internalName="MediaServiceBillingMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Notes" ma:index="27" nillable="true" ma:displayName="Notes" ma:format="Dropdown" ma:internalName="Notes">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -1676,40 +2201,26 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="17163bdb-27fe-447c-a7bb-3ea6416b971c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="451c1f4f-a267-451c-a3af-09c2fa4691f1" xsi:nil="true"/>
+    <Notes xmlns="17163bdb-27fe-447c-a7bb-3ea6416b971c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8371111F-EFF7-47C6-8985-0F43994E666C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8371111F-EFF7-47C6-8985-0F43994E666C}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{343B393C-CAC2-4750-ACA8-00CCC9C377F8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="17163bdb-27fe-447c-a7bb-3ea6416b971c"/>
-    <ds:schemaRef ds:uri="451c1f4f-a267-451c-a3af-09c2fa4691f1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D92D0016-15CA-409B-AD9C-8027C631137F}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC068CDB-1687-487F-8048-C21B0C8EEFAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="17163bdb-27fe-447c-a7bb-3ea6416b971c"/>
-    <ds:schemaRef ds:uri="451c1f4f-a267-451c-a3af-09c2fa4691f1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{343B393C-CAC2-4750-ACA8-00CCC9C377F8}"/>
 </file>
</xml_diff>

<commit_message>
Update: Rename Brand to Protocol and update template
</commit_message>
<xml_diff>
--- a/master_spreadsheet_25_26_summer.xlsx
+++ b/master_spreadsheet_25_26_summer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ysche\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yilia/Desktop/genomics-invoicing-25-26Summer-Test-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E2AD726-FCB5-4004-B499-D314F00F6CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D6F43C-59CF-2245-ABAD-2CBD164B0AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-2700" windowWidth="29040" windowHeight="15720" xr2:uid="{44EEA75D-67FD-4678-9465-A167448191E0}"/>
+    <workbookView xWindow="2840" yWindow="1640" windowWidth="25600" windowHeight="16080" xr2:uid="{44EEA75D-67FD-4678-9465-A167448191E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined Price List 25-26 Sum" sheetId="8" r:id="rId1"/>
@@ -118,9 +118,6 @@
     <t>Product Code</t>
   </si>
   <si>
-    <t>Brand</t>
-  </si>
-  <si>
     <t>Item</t>
   </si>
   <si>
@@ -371,6 +368,9 @@
   </si>
   <si>
     <t>Processing</t>
+  </si>
+  <si>
+    <t>Protocol</t>
   </si>
 </sst>
 </file>
@@ -382,7 +382,7 @@
     <numFmt numFmtId="164" formatCode="[$$-C09]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -410,7 +410,6 @@
       <sz val="11"/>
       <color rgb="FF242424"/>
       <name val="Aptos Narrow"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -624,7 +623,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1000,85 +999,85 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.625" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" customWidth="1"/>
     <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.125" customWidth="1"/>
+    <col min="4" max="4" width="36.1640625" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
-    <col min="6" max="6" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="9" customFormat="1" ht="69.95">
+    <row r="1" spans="1:10" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="I1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="J1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="9" t="s">
+    </row>
+    <row r="2" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="29.1">
-      <c r="A2" t="s">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="1">
         <v>80</v>
       </c>
       <c r="J2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="29.1">
-      <c r="A3" t="s">
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1">
         <v>100</v>
@@ -1087,287 +1086,287 @@
         <v>10</v>
       </c>
       <c r="J3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="29.1">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="F4" s="1">
         <v>20</v>
       </c>
       <c r="J4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="29.1">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="1">
         <v>50</v>
       </c>
       <c r="J5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="29.1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" s="1">
         <v>104</v>
       </c>
       <c r="J6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="29.1">
-      <c r="A7" t="s">
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="1">
         <v>1000</v>
       </c>
       <c r="J7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>32</v>
-      </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="1">
         <v>5000</v>
       </c>
       <c r="J8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="14.1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
         <v>33</v>
       </c>
-      <c r="B9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" t="s">
-        <v>34</v>
-      </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9" s="1">
         <v>5000</v>
       </c>
       <c r="J9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="29.1">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>37</v>
-      </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="1">
         <v>4500</v>
       </c>
       <c r="J10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="14.45">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>40</v>
-      </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="1">
         <v>150</v>
       </c>
       <c r="J11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="29.1">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="D12" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="1">
         <v>150</v>
       </c>
       <c r="J12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="14.1" hidden="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:10" ht="15">
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="1">
         <v>5000</v>
       </c>
       <c r="J14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="14.1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" s="1">
         <v>5000</v>
       </c>
       <c r="J15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="29.1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="1">
         <v>4500</v>
       </c>
       <c r="J16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" ht="14.45">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="1">
         <v>150</v>
       </c>
       <c r="J17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" ht="29.1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="32" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="1">
         <v>150</v>
       </c>
       <c r="J18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="4:4" ht="15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" ht="15" x14ac:dyDescent="0.2">
       <c r="D36" s="4"/>
     </row>
   </sheetData>
@@ -1394,147 +1393,147 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.375" customWidth="1"/>
-    <col min="2" max="2" width="73.375" customWidth="1"/>
-    <col min="3" max="3" width="33.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.625" customWidth="1"/>
-    <col min="5" max="5" width="11.25" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" customWidth="1"/>
+    <col min="2" max="2" width="73.33203125" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15">
-      <c r="A2" s="12" t="s">
+      <c r="B2" t="s">
         <v>51</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="8" t="s">
         <v>52</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>53</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="13">
         <v>4000</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
         <v>51</v>
       </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
       <c r="C3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="13">
         <v>5000</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="13">
         <v>500</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
         <v>51</v>
       </c>
-      <c r="B5" t="s">
-        <v>52</v>
-      </c>
       <c r="C5" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="13">
         <v>1500</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
         <v>57</v>
-      </c>
-      <c r="B6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" t="s">
-        <v>58</v>
       </c>
       <c r="E6" s="13">
         <v>2500</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
         <v>59</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="13">
         <v>5000</v>
       </c>
       <c r="F7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="14.1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="14.1">
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="E9" s="1"/>
     </row>
@@ -1552,114 +1551,114 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.25" customWidth="1"/>
-    <col min="2" max="2" width="20.375" customWidth="1"/>
-    <col min="3" max="3" width="20.625" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.1">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="18"/>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="18"/>
-    </row>
-    <row r="2" spans="1:4" ht="14.1">
-      <c r="A2" s="5" t="s">
+      <c r="B2" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="C2" s="5">
         <f>'Surcharge Editing Page'!C4</f>
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.1">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" s="5">
         <f>'Surcharge Editing Page'!D4</f>
         <v>1.3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.1">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="C4" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.1">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5">
         <f>'Surcharge Editing Page'!D8*'Config 25-26 Sum'!C4</f>
         <v>1.3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.1">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6">
         <f>C5*'Surcharge Editing Page'!E8</f>
         <v>1.885</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.1">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7">
         <f>C6*'Surcharge Editing Page'!F8</f>
         <v>2.262</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13.5" customHeight="1">
+    <row r="11" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
     </row>
-    <row r="13" spans="1:4" ht="14.1"/>
-    <row r="16" spans="1:4" ht="13.5" customHeight="1">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
     </row>
-    <row r="17" spans="1:4" ht="13.5" customHeight="1">
+    <row r="17" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="19"/>
     </row>
-    <row r="19" spans="1:4" ht="27" customHeight="1">
+    <row r="19" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="18"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
     </row>
-    <row r="20" spans="1:4" ht="13.5" customHeight="1">
+    <row r="20" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
     </row>
@@ -1676,36 +1675,36 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="17.375" customWidth="1"/>
-    <col min="3" max="3" width="15.75" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="33" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="C1" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="D1" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="23" t="s">
         <v>76</v>
-      </c>
-      <c r="E1" s="9"/>
-    </row>
-    <row r="2" spans="1:5" ht="15">
-      <c r="A2" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>77</v>
       </c>
       <c r="C2" s="23">
         <v>0.15</v>
@@ -1714,12 +1713,12 @@
         <v>45610</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" s="23">
         <v>0.2</v>
@@ -1728,12 +1727,12 @@
         <v>46009</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="23" t="s">
         <v>79</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>80</v>
       </c>
       <c r="C4" s="23">
         <v>0.18</v>
@@ -1742,12 +1741,12 @@
         <v>46034</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15">
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" s="23">
         <v>0.3</v>
@@ -1756,46 +1755,46 @@
         <v>46034</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
     </row>
-    <row r="7" spans="1:5" ht="15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="19"/>
     </row>
-    <row r="8" spans="1:5" ht="15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
     </row>
-    <row r="9" spans="1:5" ht="15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="19"/>
     </row>
-    <row r="10" spans="1:5" ht="15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
     </row>
-    <row r="11" spans="1:5" ht="15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="19"/>
     </row>
-    <row r="12" spans="1:5" ht="15">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="19"/>
     </row>
-    <row r="13" spans="1:5" ht="15">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
     </row>
-    <row r="14" spans="1:5" ht="15">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
     </row>
-    <row r="15" spans="1:5" ht="15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
     </row>
-    <row r="16" spans="1:5" ht="15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
     </row>
-    <row r="17" spans="1:1" ht="15">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="19"/>
     </row>
-    <row r="18" spans="1:1" ht="15">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="19"/>
     </row>
-    <row r="19" spans="1:1" ht="15">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="19"/>
     </row>
   </sheetData>
@@ -1812,19 +1811,19 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.625" customWidth="1"/>
-    <col min="2" max="2" width="6.625" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="11.75" customWidth="1"/>
-    <col min="6" max="6" width="12.125" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="26.1">
+    <row r="2" spans="1:6" ht="25" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -1832,21 +1831,21 @@
       <c r="E2" s="23"/>
       <c r="F2" s="23"/>
     </row>
-    <row r="3" spans="1:6" ht="15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="26" t="s">
         <v>66</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>67</v>
       </c>
       <c r="E3" s="23"/>
       <c r="F3" s="23"/>
     </row>
-    <row r="4" spans="1:6" ht="15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="23"/>
       <c r="C4" s="23">
@@ -1858,7 +1857,7 @@
       <c r="E4" s="23"/>
       <c r="F4" s="23"/>
     </row>
-    <row r="5" spans="1:6" ht="15">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="28"/>
       <c r="B5" s="23"/>
       <c r="C5" s="23"/>
@@ -1866,7 +1865,7 @@
       <c r="E5" s="23"/>
       <c r="F5" s="23"/>
     </row>
-    <row r="6" spans="1:6" ht="15">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="28"/>
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
@@ -1874,25 +1873,25 @@
       <c r="E6" s="24"/>
       <c r="F6" s="24"/>
     </row>
-    <row r="7" spans="1:6" ht="43.5">
+    <row r="7" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="28"/>
       <c r="B7" s="24"/>
       <c r="C7" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="E7" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="27" t="s">
-        <v>71</v>
-      </c>
       <c r="F7" s="27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="28" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15">
-      <c r="A8" s="28" t="s">
-        <v>85</v>
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="23">
@@ -1908,14 +1907,14 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="20"/>
     </row>
-    <row r="10" spans="1:6" ht="15">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="20"/>
       <c r="D10" s="21"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="20"/>
     </row>
   </sheetData>
@@ -1933,6 +1932,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="17163bdb-27fe-447c-a7bb-3ea6416b971c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="451c1f4f-a267-451c-a3af-09c2fa4691f1" xsi:nil="true"/>
+    <Notes xmlns="17163bdb-27fe-447c-a7bb-3ea6416b971c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009F2383067D6EEE4E8ACEA30962E5DE00" ma:contentTypeVersion="22" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0ccd53f3dd568480f5d3153c07534dba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="17163bdb-27fe-447c-a7bb-3ea6416b971c" xmlns:ns3="451c1f4f-a267-451c-a3af-09c2fa4691f1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0211ec30299ddd16592819eab657260f" ns2:_="" ns3:_="">
     <xsd:import namespace="17163bdb-27fe-447c-a7bb-3ea6416b971c"/>
@@ -2201,26 +2212,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="17163bdb-27fe-447c-a7bb-3ea6416b971c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="451c1f4f-a267-451c-a3af-09c2fa4691f1" xsi:nil="true"/>
-    <Notes xmlns="17163bdb-27fe-447c-a7bb-3ea6416b971c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8371111F-EFF7-47C6-8985-0F43994E666C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8371111F-EFF7-47C6-8985-0F43994E666C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D92D0016-15CA-409B-AD9C-8027C631137F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{343B393C-CAC2-4750-ACA8-00CCC9C377F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="17163bdb-27fe-447c-a7bb-3ea6416b971c"/>
+    <ds:schemaRef ds:uri="451c1f4f-a267-451c-a3af-09c2fa4691f1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{343B393C-CAC2-4750-ACA8-00CCC9C377F8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D92D0016-15CA-409B-AD9C-8027C631137F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="17163bdb-27fe-447c-a7bb-3ea6416b971c"/>
+    <ds:schemaRef ds:uri="451c1f4f-a267-451c-a3af-09c2fa4691f1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added new master spreadsheet
</commit_message>
<xml_diff>
--- a/master_spreadsheet_25_26_summer.xlsx
+++ b/master_spreadsheet_25_26_summer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yilia/Desktop/genomics-invoicing-25-26Summer-Test-main/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ysche\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D6F43C-59CF-2245-ABAD-2CBD164B0AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70C2790-099E-415D-9DDE-9E40954BD8E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2840" yWindow="1640" windowWidth="25600" windowHeight="16080" xr2:uid="{44EEA75D-67FD-4678-9465-A167448191E0}"/>
+    <workbookView xWindow="-28920" yWindow="-2700" windowWidth="29040" windowHeight="15720" xr2:uid="{44EEA75D-67FD-4678-9465-A167448191E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined Price List 25-26 Sum" sheetId="8" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="90">
   <si>
     <t>Product Code</t>
   </si>
@@ -139,9 +139,6 @@
     <t>Item Specific Discount</t>
   </si>
   <si>
-    <t>Platform</t>
-  </si>
-  <si>
     <t>10X-1000263</t>
   </si>
   <si>
@@ -154,18 +151,12 @@
     <t>Library &amp; Gel Bead Kit</t>
   </si>
   <si>
-    <t>Type1;Type2</t>
-  </si>
-  <si>
     <t>10X-1000265</t>
   </si>
   <si>
     <t>Chromium Next GEM Single Cell 5' Kit v2, 4 rxns</t>
   </si>
   <si>
-    <t>Type1;Type2;Type3</t>
-  </si>
-  <si>
     <t>10X-1000190</t>
   </si>
   <si>
@@ -175,9 +166,6 @@
     <t>Additional Library Kits</t>
   </si>
   <si>
-    <t>Type1</t>
-  </si>
-  <si>
     <t>10X-1000541</t>
   </si>
   <si>
@@ -190,9 +178,6 @@
     <t>Chromium Single Cell</t>
   </si>
   <si>
-    <t>ALL_PLATFORMS</t>
-  </si>
-  <si>
     <t>10X-1234572</t>
   </si>
   <si>
@@ -217,27 +202,18 @@
     <t>Chromium GEM-X Single Cell 5' Kit v3, 16 rxns</t>
   </si>
   <si>
-    <t>Type1;Type3</t>
-  </si>
-  <si>
     <t>10X-1000712</t>
   </si>
   <si>
     <t>Chromium GEM-X Single Cell 5' Kit v3, 48 rxns</t>
   </si>
   <si>
-    <t>Type2</t>
-  </si>
-  <si>
     <t>10X-1000694</t>
   </si>
   <si>
     <t>Library Construction Kit C, 16 rxns</t>
   </si>
   <si>
-    <t>Type2;Type3</t>
-  </si>
-  <si>
     <t>10X-1000703</t>
   </si>
   <si>
@@ -247,18 +223,9 @@
     <t>KBrand 775 from 10x</t>
   </si>
   <si>
-    <t>Type3</t>
-  </si>
-  <si>
-    <t>Type2;Type1</t>
-  </si>
-  <si>
     <t>Group</t>
   </si>
   <si>
-    <t>Applications (Brand)</t>
-  </si>
-  <si>
     <t>Service</t>
   </si>
   <si>
@@ -371,6 +338,51 @@
   </si>
   <si>
     <t>Protocol</t>
+  </si>
+  <si>
+    <t>Single Cell</t>
+  </si>
+  <si>
+    <t>MiniBulk</t>
+  </si>
+  <si>
+    <t>Spatial Omics</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>ALL_APPLICATIONS</t>
+  </si>
+  <si>
+    <t>MB PRM-Seq</t>
+  </si>
+  <si>
+    <t>Multiome</t>
+  </si>
+  <si>
+    <t>ALL_PROTOCOLS</t>
+  </si>
+  <si>
+    <t>5' Gene Expression;FLEX</t>
+  </si>
+  <si>
+    <t>scATACseq;3' Gene Expression</t>
+  </si>
+  <si>
+    <t>Visium v1;Visium HD</t>
+  </si>
+  <si>
+    <t>Visium HD;Visium 3' HD;Xenium</t>
+  </si>
+  <si>
+    <t>Merscope</t>
+  </si>
+  <si>
+    <t>3' Gene Expression;scPRM-Seq</t>
   </si>
 </sst>
 </file>
@@ -996,29 +1008,31 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C563ED3B-1FC1-41B6-96FD-AB3B357F4708}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.6640625" customWidth="1"/>
+    <col min="2" max="2" width="43.6328125" customWidth="1"/>
     <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.1640625" customWidth="1"/>
+    <col min="4" max="4" width="36.1796875" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
-    <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.453125" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="9" customFormat="1" ht="70" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>1</v>
@@ -1042,42 +1056,48 @@
         <v>7</v>
       </c>
       <c r="J1" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="1">
         <v>80</v>
       </c>
       <c r="J2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="1">
         <v>100</v>
@@ -1086,287 +1106,329 @@
         <v>10</v>
       </c>
       <c r="J3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="F4" s="1">
         <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+      <c r="K4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F5" s="1">
         <v>50</v>
       </c>
       <c r="J5" t="s">
+        <v>75</v>
+      </c>
+      <c r="K5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F6" s="1">
         <v>104</v>
       </c>
       <c r="J6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="K6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="1">
         <v>1000</v>
       </c>
       <c r="J7" t="s">
+        <v>76</v>
+      </c>
+      <c r="K7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
       <c r="C8" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="1">
         <v>5000</v>
       </c>
       <c r="J8" t="s">
+        <v>80</v>
+      </c>
+      <c r="K8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" s="1">
         <v>5000</v>
       </c>
       <c r="J9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="K9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>36</v>
-      </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="1">
         <v>4500</v>
       </c>
       <c r="J10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+      <c r="K10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="1">
         <v>150</v>
       </c>
       <c r="J11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="K11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="1">
         <v>150</v>
       </c>
       <c r="J12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15" hidden="1" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+      <c r="K12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="1">
         <v>5000</v>
       </c>
       <c r="J14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+      <c r="K14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" s="1">
         <v>5000</v>
       </c>
       <c r="J15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+      <c r="K15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="1">
         <v>4500</v>
       </c>
       <c r="J16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+      <c r="K16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="1">
         <v>150</v>
       </c>
       <c r="J17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" ht="32" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="K17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="1">
         <v>150</v>
       </c>
       <c r="J18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" ht="15" x14ac:dyDescent="0.35">
       <c r="D36" s="4"/>
     </row>
   </sheetData>
@@ -1387,153 +1449,175 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{890F6873-EDC7-4BE5-9189-E951DA1318D3}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.33203125" customWidth="1"/>
-    <col min="2" max="2" width="73.33203125" customWidth="1"/>
-    <col min="3" max="3" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" customWidth="1"/>
+    <col min="1" max="1" width="34.36328125" customWidth="1"/>
+    <col min="2" max="2" width="73.36328125" customWidth="1"/>
+    <col min="3" max="3" width="33.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.6328125" customWidth="1"/>
+    <col min="5" max="5" width="13.90625" customWidth="1"/>
+    <col min="6" max="6" width="19.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="13">
         <v>4000</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="G2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="13">
         <v>5000</v>
       </c>
       <c r="F3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
       <c r="C4" s="8" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="13">
         <v>500</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+      <c r="G4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="13">
         <v>1500</v>
       </c>
       <c r="F5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" t="s">
-        <v>51</v>
-      </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E6" s="13">
         <v>2500</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+      <c r="G6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="13">
         <v>5000</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+      <c r="G7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="14" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="14" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="E9" s="1"/>
     </row>
@@ -1551,114 +1635,114 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.1796875" customWidth="1"/>
+    <col min="2" max="2" width="20.36328125" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="14" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="D1" s="18"/>
     </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C2" s="5">
         <f>'Surcharge Editing Page'!C4</f>
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C3" s="5">
         <f>'Surcharge Editing Page'!D4</f>
         <v>1.3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C4" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C5">
         <f>'Surcharge Editing Page'!D8*'Config 25-26 Sum'!C4</f>
         <v>1.3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C6">
         <f>C5*'Surcharge Editing Page'!E8</f>
         <v>1.885</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C7">
         <f>C6*'Surcharge Editing Page'!F8</f>
         <v>2.262</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="19"/>
     </row>
-    <row r="17" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="19"/>
     </row>
-    <row r="19" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
     </row>
-    <row r="20" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
     </row>
@@ -1675,36 +1759,36 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="33" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="17.36328125" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" style="33" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A1" s="29" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="E1" s="9"/>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C2" s="23">
         <v>0.15</v>
@@ -1713,12 +1797,12 @@
         <v>45610</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C3" s="23">
         <v>0.2</v>
@@ -1727,12 +1811,12 @@
         <v>46009</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A4" s="22" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C4" s="23">
         <v>0.18</v>
@@ -1741,12 +1825,12 @@
         <v>46034</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C5" s="23">
         <v>0.3</v>
@@ -1755,46 +1839,46 @@
         <v>46034</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A6" s="19"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A7" s="19"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A8" s="19"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A9" s="19"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A10" s="19"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A11" s="19"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A12" s="19"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A13" s="19"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A14" s="19"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A15" s="19"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A16" s="19"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" ht="15" x14ac:dyDescent="0.35">
       <c r="A17" s="19"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" ht="15" x14ac:dyDescent="0.35">
       <c r="A18" s="19"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" ht="15" x14ac:dyDescent="0.35">
       <c r="A19" s="19"/>
     </row>
   </sheetData>
@@ -1811,19 +1895,19 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.6328125" customWidth="1"/>
+    <col min="2" max="2" width="6.6328125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" customWidth="1"/>
+    <col min="5" max="5" width="11.6328125" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="26" x14ac:dyDescent="0.6">
       <c r="A2" s="25" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -1831,21 +1915,21 @@
       <c r="E2" s="23"/>
       <c r="F2" s="23"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" s="26" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="E3" s="23"/>
       <c r="F3" s="23"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A4" s="28" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B4" s="23"/>
       <c r="C4" s="23">
@@ -1857,7 +1941,7 @@
       <c r="E4" s="23"/>
       <c r="F4" s="23"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A5" s="28"/>
       <c r="B5" s="23"/>
       <c r="C5" s="23"/>
@@ -1865,7 +1949,7 @@
       <c r="E5" s="23"/>
       <c r="F5" s="23"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A6" s="28"/>
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
@@ -1873,25 +1957,25 @@
       <c r="E6" s="24"/>
       <c r="F6" s="24"/>
     </row>
-    <row r="7" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="28"/>
       <c r="B7" s="24"/>
       <c r="C7" s="27" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A8" s="28" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="23">
@@ -1907,14 +1991,14 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A10" s="20"/>
       <c r="D10" s="21"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added updated master spreadsheet
</commit_message>
<xml_diff>
--- a/master_spreadsheet_25_26_summer.xlsx
+++ b/master_spreadsheet_25_26_summer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ysche\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70C2790-099E-415D-9DDE-9E40954BD8E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACE51F3-AE1E-44E4-93C1-E1C7235794E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2700" windowWidth="29040" windowHeight="15720" xr2:uid="{44EEA75D-67FD-4678-9465-A167448191E0}"/>
+    <workbookView xWindow="-57720" yWindow="-2700" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{44EEA75D-67FD-4678-9465-A167448191E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined Price List 25-26 Sum" sheetId="8" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="96">
   <si>
     <t>Product Code</t>
   </si>
@@ -383,6 +383,24 @@
   </si>
   <si>
     <t>3' Gene Expression;scPRM-Seq</t>
+  </si>
+  <si>
+    <t>Discount Type</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Gem-X3 Discount</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Kbrand</t>
+  </si>
+  <si>
+    <t>K-1 Discount</t>
   </si>
 </sst>
 </file>
@@ -394,7 +412,7 @@
     <numFmt numFmtId="164" formatCode="[$$-C09]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1010,11 +1028,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="K2" sqref="K2:K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.6328125" customWidth="1"/>
@@ -1027,7 +1045,7 @@
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="9" customFormat="1" ht="70" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="9" customFormat="1" ht="70">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1062,7 +1080,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="29">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1086,7 +1104,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="29">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1112,7 +1130,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="29">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -1135,7 +1153,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="29">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -1158,7 +1176,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="29">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
@@ -1181,7 +1199,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="29">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1205,7 +1223,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="15">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1229,7 +1247,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="14">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1252,7 +1270,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="29">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1276,7 +1294,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="14.5">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1300,7 +1318,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="29">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1324,10 +1342,10 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="14" hidden="1">
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="15">
       <c r="B14" t="s">
         <v>35</v>
       </c>
@@ -1348,7 +1366,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="14">
       <c r="B15" t="s">
         <v>35</v>
       </c>
@@ -1368,7 +1386,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="29">
       <c r="B16" t="s">
         <v>35</v>
       </c>
@@ -1389,7 +1407,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" ht="14.5">
       <c r="B17" t="s">
         <v>35</v>
       </c>
@@ -1410,7 +1428,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:11" ht="29">
       <c r="B18" t="s">
         <v>35</v>
       </c>
@@ -1428,7 +1446,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="4:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:4" ht="15">
       <c r="D36" s="4"/>
     </row>
   </sheetData>
@@ -1455,7 +1473,7 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="34.36328125" customWidth="1"/>
     <col min="2" max="2" width="73.36328125" customWidth="1"/>
@@ -1465,7 +1483,7 @@
     <col min="6" max="6" width="19.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15">
       <c r="A1" s="11" t="s">
         <v>36</v>
       </c>
@@ -1488,7 +1506,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="15">
       <c r="A2" s="12" t="s">
         <v>39</v>
       </c>
@@ -1509,7 +1527,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="15">
       <c r="A3" s="12" t="s">
         <v>39</v>
       </c>
@@ -1530,7 +1548,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="15">
       <c r="A4" s="12" t="s">
         <v>39</v>
       </c>
@@ -1551,7 +1569,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="15">
       <c r="A5" s="12" t="s">
         <v>39</v>
       </c>
@@ -1572,7 +1590,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="15">
       <c r="A6" s="12" t="s">
         <v>45</v>
       </c>
@@ -1592,7 +1610,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="15">
       <c r="A7" s="12" t="s">
         <v>47</v>
       </c>
@@ -1613,11 +1631,11 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="14">
       <c r="A8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:7" ht="14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="14">
       <c r="A9" s="1"/>
       <c r="E9" s="1"/>
     </row>
@@ -1635,14 +1653,14 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="19.1796875" customWidth="1"/>
     <col min="2" max="2" width="20.36328125" customWidth="1"/>
     <col min="3" max="3" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="14">
       <c r="A1" s="9" t="s">
         <v>50</v>
       </c>
@@ -1654,7 +1672,7 @@
       </c>
       <c r="D1" s="18"/>
     </row>
-    <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="14">
       <c r="A2" s="5" t="s">
         <v>53</v>
       </c>
@@ -1666,7 +1684,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="14">
       <c r="A3" s="5" t="s">
         <v>53</v>
       </c>
@@ -1678,7 +1696,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="14">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -1689,7 +1707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="14">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -1701,7 +1719,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="14">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -1713,7 +1731,7 @@
         <v>1.885</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="14">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -1725,24 +1743,24 @@
         <v>2.262</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="13.5" customHeight="1">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
     </row>
-    <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="14"/>
+    <row r="16" spans="1:4" ht="13.5" customHeight="1">
       <c r="A16" s="19"/>
     </row>
-    <row r="17" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="13.5" customHeight="1">
       <c r="A17" s="19"/>
     </row>
-    <row r="19" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="27" customHeight="1">
       <c r="A19" s="18"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
     </row>
-    <row r="20" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="13.5" customHeight="1">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
     </row>
@@ -1755,11 +1773,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E225A74-4726-489B-BA52-DC430EC611A1}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView zoomScale="197" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="197" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="17.36328125" customWidth="1"/>
@@ -1768,7 +1786,7 @@
     <col min="5" max="5" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15">
       <c r="A1" s="29" t="s">
         <v>61</v>
       </c>
@@ -1781,9 +1799,11 @@
       <c r="D1" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="9"/>
-    </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="E1" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15">
       <c r="A2" s="22" t="s">
         <v>46</v>
       </c>
@@ -1796,8 +1816,11 @@
       <c r="D2" s="32">
         <v>45610</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15">
       <c r="A3" s="22" t="s">
         <v>46</v>
       </c>
@@ -1810,8 +1833,11 @@
       <c r="D3" s="32">
         <v>46009</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15">
       <c r="A4" s="22" t="s">
         <v>67</v>
       </c>
@@ -1824,8 +1850,11 @@
       <c r="D4" s="32">
         <v>46034</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="E4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15">
       <c r="A5" s="22" t="s">
         <v>67</v>
       </c>
@@ -1838,47 +1867,78 @@
       <c r="D5" s="32">
         <v>46034</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A6" s="19"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A7" s="19"/>
-    </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="E5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15">
+      <c r="A6" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="23">
+        <v>45</v>
+      </c>
+      <c r="D6" s="32">
+        <v>46034</v>
+      </c>
+      <c r="E6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15">
+      <c r="A7" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="23">
+        <v>200</v>
+      </c>
+      <c r="D7" s="33">
+        <v>46388</v>
+      </c>
+      <c r="E7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15">
       <c r="A8" s="19"/>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="15">
       <c r="A9" s="19"/>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="15">
       <c r="A10" s="19"/>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="15">
       <c r="A11" s="19"/>
     </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="15">
       <c r="A12" s="19"/>
     </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="15">
       <c r="A13" s="19"/>
     </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="15">
       <c r="A14" s="19"/>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="15">
       <c r="A15" s="19"/>
     </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="15">
       <c r="A16" s="19"/>
     </row>
-    <row r="17" spans="1:1" ht="15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" ht="15">
       <c r="A17" s="19"/>
     </row>
-    <row r="18" spans="1:1" ht="15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" ht="15">
       <c r="A18" s="19"/>
     </row>
-    <row r="19" spans="1:1" ht="15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" ht="15">
       <c r="A19" s="19"/>
     </row>
   </sheetData>
@@ -1895,7 +1955,7 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="19.6328125" customWidth="1"/>
     <col min="2" max="2" width="6.6328125" customWidth="1"/>
@@ -1905,7 +1965,7 @@
     <col min="6" max="6" width="12.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="26" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:6" ht="26">
       <c r="A2" s="25" t="s">
         <v>70</v>
       </c>
@@ -1915,7 +1975,7 @@
       <c r="E2" s="23"/>
       <c r="F2" s="23"/>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" s="26" t="s">
@@ -1927,7 +1987,7 @@
       <c r="E3" s="23"/>
       <c r="F3" s="23"/>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15">
       <c r="A4" s="28" t="s">
         <v>71</v>
       </c>
@@ -1941,7 +2001,7 @@
       <c r="E4" s="23"/>
       <c r="F4" s="23"/>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15">
       <c r="A5" s="28"/>
       <c r="B5" s="23"/>
       <c r="C5" s="23"/>
@@ -1949,7 +2009,7 @@
       <c r="E5" s="23"/>
       <c r="F5" s="23"/>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15">
       <c r="A6" s="28"/>
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
@@ -1957,7 +2017,7 @@
       <c r="E6" s="24"/>
       <c r="F6" s="24"/>
     </row>
-    <row r="7" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="43.5">
       <c r="A7" s="28"/>
       <c r="B7" s="24"/>
       <c r="C7" s="27" t="s">
@@ -1973,7 +2033,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15">
       <c r="A8" s="28" t="s">
         <v>73</v>
       </c>
@@ -1991,14 +2051,14 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="20"/>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15">
       <c r="A10" s="20"/>
       <c r="D10" s="21"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="20"/>
     </row>
   </sheetData>

</xml_diff>